<commit_message>
fix_import_data、fix_memberRegisterVerify update runAll _reportTitle for AB007
</commit_message>
<xml_diff>
--- a/test_data/document/memberSearchBatch.xlsx
+++ b/test_data/document/memberSearchBatch.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\automation_test_project\test_data\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,21 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>帐号</t>
-  </si>
-  <si>
-    <t>DS</t>
   </si>
   <si>
     <t>DS_player4</t>
   </si>
   <si>
     <t>DS_player8</t>
-  </si>
-  <si>
-    <t>DS_player7</t>
   </si>
 </sst>
 </file>
@@ -351,11 +345,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,16 +372,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>